<commit_message>
added fields segment, state, city, country for customer details
</commit_message>
<xml_diff>
--- a/LittleLemonDB.xlsx
+++ b/LittleLemonDB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdiel Chiu\Documents\Universidades\Open Source Computer Science Degree\Database Engineer Certification by META\8. Database Engineer Capstone\Excel Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8D25B1-5BB3-44DE-A220-DEA999FE3F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2642CA-ECEB-4CF4-9473-68F684137B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bookings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="146">
   <si>
     <t>booking_id</t>
   </si>
@@ -348,6 +348,126 @@
   </si>
   <si>
     <t>staff_id</t>
+  </si>
+  <si>
+    <t>Consumer</t>
+  </si>
+  <si>
+    <t>New York City</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Corporate</t>
+  </si>
+  <si>
+    <t>Wollongong</t>
+  </si>
+  <si>
+    <t>New South Wales</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Brisbane</t>
+  </si>
+  <si>
+    <t>Queensland</t>
+  </si>
+  <si>
+    <t>Home Office</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Dakar</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>Porirua</t>
+  </si>
+  <si>
+    <t>Wellington</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>Hamilton</t>
+  </si>
+  <si>
+    <t>Waikato</t>
+  </si>
+  <si>
+    <t>Sacramento</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Concord</t>
+  </si>
+  <si>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>Alexandria</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>Kabul</t>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>Jizan</t>
+  </si>
+  <si>
+    <t>Saudi Arabia</t>
+  </si>
+  <si>
+    <t>Toledo</t>
+  </si>
+  <si>
+    <t>Parana</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Segment</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Henderson</t>
+  </si>
+  <si>
+    <t>Kentucky</t>
   </si>
 </sst>
 </file>
@@ -383,9 +503,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -922,19 +1044,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFDCC86F-773B-415D-8995-AE88AE7131DA}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -944,8 +1067,20 @@
       <c r="C1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -955,8 +1090,20 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -966,8 +1113,20 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -977,8 +1136,20 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -988,8 +1159,20 @@
       <c r="C5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -999,8 +1182,20 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1010,8 +1205,20 @@
       <c r="C7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1021,8 +1228,20 @@
       <c r="C8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1032,8 +1251,20 @@
       <c r="C9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1043,8 +1274,20 @@
       <c r="C10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D10" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1054,8 +1297,20 @@
       <c r="C11" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D11" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1065,8 +1320,20 @@
       <c r="C12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D12" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1076,8 +1343,20 @@
       <c r="C13" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D13" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1087,8 +1366,20 @@
       <c r="C14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D14" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1098,8 +1389,20 @@
       <c r="C15" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D15" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1108,6 +1411,18 @@
       </c>
       <c r="C16" t="s">
         <v>35</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1893,7 +2208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BE61D99-C358-47A8-BB81-0F98BF6EACD7}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added staff information table
</commit_message>
<xml_diff>
--- a/LittleLemonDB.xlsx
+++ b/LittleLemonDB.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdiel Chiu\Documents\Universidades\Open Source Computer Science Degree\Database Engineer Certification by META\8. Database Engineer Capstone\Excel Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2642CA-ECEB-4CF4-9473-68F684137B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9DB61DC-30C8-4D7A-B8EA-48AF5CA91A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23730" yWindow="2120" windowWidth="14400" windowHeight="13570" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bookings" sheetId="1" r:id="rId1"/>
     <sheet name="customer_details" sheetId="2" r:id="rId2"/>
-    <sheet name="menu" sheetId="3" r:id="rId3"/>
-    <sheet name="menuitems" sheetId="4" r:id="rId4"/>
-    <sheet name="order_delivery_status" sheetId="6" r:id="rId5"/>
-    <sheet name="orders" sheetId="7" r:id="rId6"/>
+    <sheet name="staff_information" sheetId="8" r:id="rId3"/>
+    <sheet name="menu" sheetId="3" r:id="rId4"/>
+    <sheet name="menuitems" sheetId="4" r:id="rId5"/>
+    <sheet name="order_delivery_status" sheetId="6" r:id="rId6"/>
+    <sheet name="orders" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="164">
   <si>
     <t>booking_id</t>
   </si>
@@ -468,6 +469,60 @@
   </si>
   <si>
     <t>Kentucky</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>salary</t>
+  </si>
+  <si>
+    <t>hire_date</t>
+  </si>
+  <si>
+    <t>Waiter</t>
+  </si>
+  <si>
+    <t>Chef</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Bartender</t>
+  </si>
+  <si>
+    <t>Host/Hostess</t>
+  </si>
+  <si>
+    <t>Sous Chef</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>Dishwasher</t>
+  </si>
+  <si>
+    <t>Line Cook</t>
+  </si>
+  <si>
+    <t>Busser</t>
+  </si>
+  <si>
+    <t>Food Runner</t>
+  </si>
+  <si>
+    <t>Prep Cook</t>
+  </si>
+  <si>
+    <t>Head Chef</t>
+  </si>
+  <si>
+    <t>Floor Manager</t>
+  </si>
+  <si>
+    <t>Sommelier</t>
   </si>
 </sst>
 </file>
@@ -503,11 +558,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1046,7 +1099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFDCC86F-773B-415D-8995-AE88AE7131DA}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -1067,16 +1120,16 @@
       <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>140</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>141</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>142</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>143</v>
       </c>
     </row>
@@ -1090,16 +1143,16 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>106</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>107</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>108</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1113,16 +1166,16 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>110</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" t="s">
         <v>111</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" t="s">
         <v>112</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1136,16 +1189,16 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>106</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" t="s">
         <v>114</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" t="s">
         <v>115</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1159,16 +1212,16 @@
       <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>116</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" t="s">
         <v>117</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" t="s">
         <v>117</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1182,16 +1235,16 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>106</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" t="s">
         <v>119</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" t="s">
         <v>119</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1205,16 +1258,16 @@
       <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s">
         <v>110</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" t="s">
         <v>121</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" t="s">
         <v>112</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1228,16 +1281,16 @@
       <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" t="s">
         <v>106</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" t="s">
         <v>122</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" t="s">
         <v>123</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1251,16 +1304,16 @@
       <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" t="s">
         <v>106</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" t="s">
         <v>125</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" t="s">
         <v>126</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1274,16 +1327,16 @@
       <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" t="s">
         <v>110</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" t="s">
         <v>127</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" t="s">
         <v>128</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1297,16 +1350,16 @@
       <c r="C11" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" t="s">
         <v>106</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" t="s">
         <v>129</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" t="s">
         <v>130</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1320,16 +1373,16 @@
       <c r="C12" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" t="s">
         <v>110</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" t="s">
         <v>131</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" t="s">
         <v>132</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1343,16 +1396,16 @@
       <c r="C13" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" t="s">
         <v>110</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" t="s">
         <v>133</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" t="s">
         <v>133</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1366,16 +1419,16 @@
       <c r="C14" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" t="s">
         <v>106</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" t="s">
         <v>135</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" t="s">
         <v>135</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" t="s">
         <v>136</v>
       </c>
     </row>
@@ -1389,16 +1442,16 @@
       <c r="C15" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" t="s">
         <v>116</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" t="s">
         <v>137</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" t="s">
         <v>138</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" t="s">
         <v>139</v>
       </c>
     </row>
@@ -1412,16 +1465,16 @@
       <c r="C16" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" t="s">
         <v>110</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" t="s">
         <v>144</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" t="s">
         <v>145</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1431,6 +1484,248 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47183308-8B6D-4A02-A737-8FA9488E482A}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2">
+        <v>2000</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44562</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3">
+        <v>3000</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44576</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4">
+        <v>4000</v>
+      </c>
+      <c r="D4" s="1">
+        <v>44593</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5">
+        <v>2500</v>
+      </c>
+      <c r="D5" s="1">
+        <v>44607</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6">
+        <v>1800</v>
+      </c>
+      <c r="D6" s="1">
+        <v>44621</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7">
+        <v>3200</v>
+      </c>
+      <c r="D7" s="1">
+        <v>44635</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8">
+        <v>2000</v>
+      </c>
+      <c r="D8" s="1">
+        <v>44652</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9">
+        <v>1800</v>
+      </c>
+      <c r="D9" s="1">
+        <v>44666</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10">
+        <v>2400</v>
+      </c>
+      <c r="D10" s="1">
+        <v>44682</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>158</v>
+      </c>
+      <c r="C11">
+        <v>1700</v>
+      </c>
+      <c r="D11" s="1">
+        <v>44696</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C12">
+        <v>1700</v>
+      </c>
+      <c r="D12" s="1">
+        <v>44713</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13">
+        <v>2000</v>
+      </c>
+      <c r="D13" s="1">
+        <v>44727</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>161</v>
+      </c>
+      <c r="C14">
+        <v>4000</v>
+      </c>
+      <c r="D14" s="1">
+        <v>44743</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>162</v>
+      </c>
+      <c r="C15">
+        <v>3500</v>
+      </c>
+      <c r="D15" s="1">
+        <v>44757</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>163</v>
+      </c>
+      <c r="C16">
+        <v>3000</v>
+      </c>
+      <c r="D16" s="1">
+        <v>44774</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FFA03B4-569D-4E0E-B8D5-137952241C6A}">
   <dimension ref="A1:E16"/>
   <sheetViews>
@@ -1717,7 +2012,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314F811B-1554-4203-BCD8-B61F1FABE781}">
   <dimension ref="A1:D16"/>
   <sheetViews>
@@ -1962,7 +2257,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB14817-9214-43EC-B88A-04EAD355F14F}">
   <dimension ref="A1:D16"/>
   <sheetViews>
@@ -2204,7 +2499,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BE61D99-C358-47A8-BB81-0F98BF6EACD7}">
   <dimension ref="A1:H16"/>
   <sheetViews>

</xml_diff>